<commit_message>
v0.23 Page per etappe
</commit_message>
<xml_diff>
--- a/tdf-current.xlsx
+++ b/tdf-current.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\Tourploeg\Claude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A4CD0A-0CFC-4C1A-A83C-0F2E77827AFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7151796A-C336-4FA0-940C-97F00EAD3382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{C407EA6E-0DA1-4649-9E9C-17974BBC531D}"/>
   </bookViews>
@@ -3966,8 +3966,8 @@
   <sheetPr codeName="Blad4"/>
   <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B30" sqref="A1:B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3978,7 +3978,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>129</v>
+        <v>240</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>130</v>

</xml_diff>